<commit_message>
AD3-374 All admin forms with English and French fields
</commit_message>
<xml_diff>
--- a/forms/src/main/resources/org/devgateway/toolkit/forms/wicket/page/edit/productionDataset-Template.xlsx
+++ b/forms/src/main/resources/org/devgateway/toolkit/forms/wicket/page/edit/productionDataset-Template.xlsx
@@ -24,7 +24,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t xml:space="preserve">Region</t>
+    <t xml:space="preserve">Department</t>
   </si>
   <si>
     <t xml:space="preserve">Campaing</t>
@@ -229,7 +229,7 @@
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -243,7 +243,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
AD3-205 Typos throughout the application
</commit_message>
<xml_diff>
--- a/forms/src/main/resources/org/devgateway/toolkit/forms/wicket/page/edit/productionDataset-Template.xlsx
+++ b/forms/src/main/resources/org/devgateway/toolkit/forms/wicket/page/edit/productionDataset-Template.xlsx
@@ -22,12 +22,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t xml:space="preserve">Department</t>
   </si>
   <si>
-    <t xml:space="preserve">Year</t>
+    <t xml:space="preserve">Campaign</t>
   </si>
   <si>
     <t xml:space="preserve">Crop</t>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t xml:space="preserve">Bakel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017/2018</t>
   </si>
   <si>
     <t xml:space="preserve">Corn</t>
@@ -431,7 +434,7 @@
   <dimension ref="A1:L46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C2:C20"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -445,7 +448,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -475,282 +478,285 @@
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="C2" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -772,7 +778,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C2:C20 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -798,7 +804,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C2:C20 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>